<commit_message>
Going on with the scenarios
Pour que Louise puisse l'utiliser en python
</commit_message>
<xml_diff>
--- a/correspondances_variables.xlsx
+++ b/correspondances_variables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="231">
   <si>
     <t>id_indiv</t>
   </si>
@@ -597,6 +597,141 @@
   </si>
   <si>
     <t>Loyer mensuel</t>
+  </si>
+  <si>
+    <t>Intérêts et autre revenus assimilés  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus values </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenus fonciers </t>
+  </si>
+  <si>
+    <t>f2dc</t>
+  </si>
+  <si>
+    <t>f2tr</t>
+  </si>
+  <si>
+    <t>f3vg</t>
+  </si>
+  <si>
+    <t>f4ba</t>
+  </si>
+  <si>
+    <t>Case 2042</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>f2ts</t>
+  </si>
+  <si>
+    <t>f2go</t>
+  </si>
+  <si>
+    <t>Revenus de valeurs mobilières et distributions</t>
+  </si>
+  <si>
+    <t>Autres revenus distribués et revenus des structures soumises hors de France à un régime fiscal privilégié</t>
+  </si>
+  <si>
+    <t>Intérêts imposés au barème</t>
+  </si>
+  <si>
+    <t>Revenus imposables des titres non côtés détenus dans le PEA et distributions perçues via votre entreprise donnant droit à abattement</t>
+  </si>
+  <si>
+    <t>f2fu</t>
+  </si>
+  <si>
+    <t>Revenus des actions et parts donnant droit à abattement</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>Dividendes imposés au barème</t>
+  </si>
+  <si>
+    <t>Plus-values mobilières (regime normal)</t>
+  </si>
+  <si>
+    <t>Revenus fonciers (régime normal) (=case BA)</t>
+  </si>
+  <si>
+    <t>Retraite imposable</t>
+  </si>
+  <si>
+    <t>Chômage imposable</t>
+  </si>
+  <si>
+    <t>activite</t>
+  </si>
+  <si>
+    <t>absent mais imputable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    </t>
+  </si>
+  <si>
+    <t>Enum([u'Actif occupé',  u'Chômeur', u'Étudiant, élève',u'Retraité', u'Autre inactif']), default = 4)),</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>caseT</t>
+  </si>
+  <si>
+    <t>Vous êtes parent isolé au 1er janvier de l'année n-1</t>
+  </si>
+  <si>
+    <t>Personne vivant seule avec des enfants 0-1 (=case T décl. 2042)</t>
+  </si>
+  <si>
+    <t>Personne vivant seule ayant eu des enfants aujourd’hui majeurs ou décédés (=case E-K-L déclaration 2042)</t>
+  </si>
+  <si>
+    <t>caseE</t>
+  </si>
+  <si>
+    <t>caseK</t>
+  </si>
+  <si>
+    <t>caseL</t>
+  </si>
+  <si>
+    <t>Situation pouvant donner droit à une demi-part supplémentaire: enfant élevé seul pendant moins de 5 ans</t>
+  </si>
+  <si>
+    <t>Situation pouvant donner droit à une demi-part supplémentaire: vous avez eu un enfant décédé après l’âge de 16 ans ou par suite de faits de guerre</t>
+  </si>
+  <si>
+    <t>Situation pouvant donner droit à une demi-part supplémentaire: enfant élevé seul pendant plus de 5 ans</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -744,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -809,6 +944,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -822,6 +960,19 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1125,26 +1276,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="5"/>
-    <col min="5" max="5" width="50.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="44.42578125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" style="5"/>
+    <col min="6" max="6" width="50.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>154</v>
       </c>
@@ -1155,569 +1309,799 @@
         <v>155</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>160</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="21" t="s">
+      <c r="H2" s="6"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="21" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="28"/>
+      <c r="K3" s="17" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="18" t="s">
+      <c r="H4" s="6"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="11"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="11"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="11"/>
+      <c r="E12" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>173</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="G13" s="25" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="23"/>
+      <c r="H13" s="25" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="11"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="11"/>
+      <c r="E15" s="3">
         <v>7</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="F15" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="F16" s="10" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="G17" s="10" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="3"/>
+      <c r="H17" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="3"/>
+      <c r="F18" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="10" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H19" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="10" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20"/>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="E22" s="3"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" t="s">
+        <v>215</v>
+      </c>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="E27" s="3"/>
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27"/>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28"/>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29"/>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32"/>
+      <c r="E32" s="3"/>
       <c r="F32"/>
+      <c r="G32"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33"/>
+        <v>43</v>
+      </c>
+      <c r="E33" s="3"/>
       <c r="F33"/>
+      <c r="G33"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34"/>
+        <v>44</v>
+      </c>
+      <c r="E34" s="3"/>
       <c r="F34"/>
+      <c r="G34"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35"/>
+        <v>45</v>
+      </c>
+      <c r="E35" s="3"/>
       <c r="F35"/>
+      <c r="G35"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36"/>
+        <v>46</v>
+      </c>
+      <c r="E36" s="3"/>
       <c r="F36"/>
+      <c r="G36"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="31"/>
+      <c r="C41" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="31"/>
+      <c r="C42" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="G39" s="13" t="s">
+      <c r="B45" s="35"/>
+      <c r="C45" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="F45" s="32"/>
+      <c r="G45" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" t="s">
+        <v>194</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="36"/>
+      <c r="C47" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="F47" s="31"/>
+      <c r="G47" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D49" s="33"/>
+      <c r="F49" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" s="33"/>
+      <c r="F50" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C53" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="G42" s="19" t="s">
+      <c r="D53" s="11"/>
+      <c r="E53" s="3"/>
+      <c r="H53" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="G43" s="19" t="s">
+      <c r="E54" s="3"/>
+      <c r="H54" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="I54" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C56" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="G45" s="13" t="s">
+      <c r="D56" s="11"/>
+      <c r="E56" s="3"/>
+      <c r="G56" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="H56" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C57" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="G46" s="13" t="s">
+      <c r="D57" s="11"/>
+      <c r="E57" s="3"/>
+      <c r="G57" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="H57" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="C47" s="10" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="10"/>
+      <c r="C58" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="D47" s="24"/>
-      <c r="F47" s="10" t="s">
+      <c r="D58" s="10"/>
+      <c r="E58" s="24"/>
+      <c r="G58" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49" s="2"/>
-      <c r="F49"/>
-      <c r="G49"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60" s="2"/>
+      <c r="G60"/>
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C61" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D61" s="26"/>
+      <c r="E61" s="5">
         <v>1</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F61" t="s">
         <v>180</v>
       </c>
-      <c r="G50"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="5">
+      <c r="C62" s="31"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="5">
         <v>2</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F62" t="s">
         <v>174</v>
       </c>
-      <c r="G51"/>
-      <c r="I51" s="30" t="s">
+      <c r="H62"/>
+      <c r="J62" s="31" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="5" t="s">
+      <c r="C63" s="31"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F63" t="s">
         <v>175</v>
       </c>
-      <c r="G52"/>
-      <c r="I52" s="30"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="H63"/>
+      <c r="J63" s="31"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="5">
+      <c r="C64" s="31"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="5">
         <v>6</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F64" t="s">
         <v>176</v>
       </c>
-      <c r="G53"/>
-      <c r="I53" s="30"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="H64"/>
+      <c r="J64" s="31"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>117</v>
       </c>
-      <c r="D54"/>
-      <c r="E54" t="s">
+      <c r="E65"/>
+      <c r="F65" t="s">
         <v>178</v>
       </c>
-      <c r="G54"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>118</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C66" t="s">
         <v>184</v>
       </c>
-      <c r="D55"/>
-      <c r="E55" t="s">
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66" t="s">
         <v>179</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="G66" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G55"/>
+      <c r="H66"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I1:I4"/>
+  <mergeCells count="10">
+    <mergeCell ref="J1:J4"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="J62:J64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="F40:F42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some database from TAXIPP + update Programme_IPP.do
Les noms des bases sont sensées expliciter le contenu du scenario !
</commit_message>
<xml_diff>
--- a/correspondances_variables.xlsx
+++ b/correspondances_variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="14955" windowHeight="12855"/>
+    <workbookView xWindow="-30" yWindow="30" windowWidth="14955" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight" activeCell="F40" sqref="F40:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,10 +1714,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="11" t="s">
         <v>218</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -1732,10 +1732,10 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="11" t="s">
         <v>222</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -1750,8 +1750,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="31"/>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="36"/>
+      <c r="C41" s="11" t="s">
         <v>223</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -1764,8 +1764,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="31"/>
-      <c r="C42" s="5" t="s">
+      <c r="B42" s="36"/>
+      <c r="C42" s="11" t="s">
         <v>224</v>
       </c>
       <c r="D42" s="5" t="s">

</xml_diff>